<commit_message>
Added all test classes and updated all pages
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,13 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15855" windowHeight="2310"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Meal Search Results" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Meals" sheetId="2" r:id="rId5"/>
+    <sheet name="Meal Search Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Meals" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519"/>
+  <oleSize ref="A7:G12"/>
 </workbook>
 </file>
 
@@ -134,27 +138,34 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="5">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -162,7 +173,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -172,51 +183,38 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -406,27 +404,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:X22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.86"/>
-    <col customWidth="1" min="2" max="2" width="25.86"/>
-    <col customWidth="1" min="3" max="3" width="22.29"/>
-    <col customWidth="1" min="4" max="4" width="19.43"/>
-    <col customWidth="1" min="5" max="5" width="18.71"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:24">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -445,7 +448,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -460,7 +463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:24">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -468,7 +471,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
@@ -477,7 +480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:24">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -485,13 +488,13 @@
         <v>13</v>
       </c>
       <c r="C4" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:24">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -499,10 +502,10 @@
         <v>15</v>
       </c>
       <c r="C5" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -510,7 +513,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>7</v>
@@ -519,7 +522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:24">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -527,7 +530,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="3">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>5</v>
@@ -593,115 +596,116 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:24">
       <c r="B8" s="5"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:24">
       <c r="B9" s="5"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:24">
       <c r="B10" s="5"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:24">
       <c r="B11" s="5"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:24">
       <c r="B12" s="5"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:24">
       <c r="B13" s="5"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:24">
       <c r="B14" s="5"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:24">
       <c r="B15" s="5"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:24">
       <c r="B16" s="5"/>
     </row>
-    <row r="17">
+    <row r="17" spans="2:2">
       <c r="B17" s="5"/>
     </row>
-    <row r="18">
+    <row r="18" spans="2:2">
       <c r="B18" s="5"/>
     </row>
-    <row r="19">
+    <row r="19" spans="2:2">
       <c r="B19" s="5"/>
     </row>
-    <row r="20">
+    <row r="20" spans="2:2">
       <c r="B20" s="5"/>
     </row>
-    <row r="21">
+    <row r="21" spans="2:2">
       <c r="B21" s="5"/>
     </row>
-    <row r="22">
+    <row r="22" spans="2:2">
       <c r="B22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B6"/>
-    <hyperlink r:id="rId6" ref="B7"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
   </hyperlinks>
-  <drawing r:id="rId7"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="56.29"/>
+    <col min="1" max="1" width="56.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1">
       <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:1">
       <c r="A4" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:1">
       <c r="A6" s="6" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
-    <hyperlink r:id="rId2" ref="A3"/>
-    <hyperlink r:id="rId3" ref="A4"/>
-    <hyperlink r:id="rId4" ref="A5"/>
-    <hyperlink r:id="rId5" ref="A6"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
-  <drawing r:id="rId6"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>